<commit_message>
update 27 June 2021
</commit_message>
<xml_diff>
--- a/tables/2021-06/sup_table_overview_Jun.xlsx
+++ b/tables/2021-06/sup_table_overview_Jun.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="252">
   <si>
     <t>Population size</t>
   </si>
@@ -704,13 +704,7 @@
     <t>17.1 (9.2-28.0)</t>
   </si>
   <si>
-    <t>1.5 (0.9-2.2)</t>
-  </si>
-  <si>
-    <t>0.5 (0.1-1.8)</t>
-  </si>
-  <si>
-    <t>0.6 (0.0-3.4)</t>
+    <t>1.7 (1.1-2.4)</t>
   </si>
   <si>
     <t>0.7 (0.0-4.0)</t>
@@ -722,7 +716,7 @@
     <t>1.1 (0.1-3.8)</t>
   </si>
   <si>
-    <t>0.5 (0.1-2.0)</t>
+    <t>0.8 (0.2-2.4)</t>
   </si>
   <si>
     <t>0.7 (0.1-2.1)</t>
@@ -737,13 +731,13 @@
     <t>20.0 (11.4-31.3)</t>
   </si>
   <si>
-    <t>4.1 (3.2-5.2)</t>
-  </si>
-  <si>
-    <t>7.0 (4.7-10.0)</t>
-  </si>
-  <si>
-    <t>9.1 (5.2-14.6)</t>
+    <t>3.9 (3.0-5.0)</t>
+  </si>
+  <si>
+    <t>6.5 (4.3-9.4)</t>
+  </si>
+  <si>
+    <t>7.9 (4.3-13.2)</t>
   </si>
   <si>
     <t>8.8 (4.6-14.9)</t>
@@ -758,10 +752,7 @@
     <t>5.9 (3.0-10.3)</t>
   </si>
   <si>
-    <t>1.6 (0.6-3.6)</t>
-  </si>
-  <si>
-    <t>2.8 (0.3-9.7)</t>
+    <t>1.4 (0.4-3.2)</t>
   </si>
   <si>
     <t>1.6 (0.0-8.4)</t>
@@ -949,16 +940,16 @@
         <v>203</v>
       </c>
       <c r="S2" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="T2" t="s">
         <v>230</v>
       </c>
       <c r="U2" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="V2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
@@ -1017,16 +1008,16 @@
         <v>204</v>
       </c>
       <c r="S3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="T3" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="U3" t="n">
-        <v>28.0</v>
+        <v>26.0</v>
       </c>
       <c r="V3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4">
@@ -1085,16 +1076,16 @@
         <v>205</v>
       </c>
       <c r="S4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="T4" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="U4" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="V4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
@@ -1224,13 +1215,13 @@
         <v>1.0</v>
       </c>
       <c r="T6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U6" t="n">
         <v>12.0</v>
       </c>
       <c r="V6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7">
@@ -1298,7 +1289,7 @@
         <v>1.0</v>
       </c>
       <c r="V7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8">
@@ -1360,13 +1351,13 @@
         <v>2.0</v>
       </c>
       <c r="T8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="U8" t="n">
         <v>11.0</v>
       </c>
       <c r="V8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9">
@@ -1428,13 +1419,13 @@
         <v>2.0</v>
       </c>
       <c r="T9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="U9" t="n">
         <v>11.0</v>
       </c>
       <c r="V9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10">
@@ -1629,16 +1620,16 @@
         <v>212</v>
       </c>
       <c r="S12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="T12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="U12" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="V12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13">
@@ -1697,16 +1688,16 @@
         <v>213</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T13" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="U13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="V13" t="s">
-        <v>249</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14">
@@ -1978,7 +1969,7 @@
         <v>1.0</v>
       </c>
       <c r="V17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18">
@@ -2250,7 +2241,7 @@
         <v>1.0</v>
       </c>
       <c r="V21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22">
@@ -2448,7 +2439,7 @@
         <v>3.0</v>
       </c>
       <c r="T24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="U24" t="n">
         <v>13.0</v>
@@ -2862,7 +2853,7 @@
         <v>2.0</v>
       </c>
       <c r="V30" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31">
@@ -2924,13 +2915,13 @@
         <v>3.0</v>
       </c>
       <c r="T31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="U31" t="n">
         <v>9.0</v>
       </c>
       <c r="V31" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32">
@@ -2992,13 +2983,13 @@
         <v>14.0</v>
       </c>
       <c r="T32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="U32" t="n">
         <v>3.0</v>
       </c>
       <c r="V32" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33">
@@ -3128,13 +3119,13 @@
         <v>14.0</v>
       </c>
       <c r="T34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="U34" t="n">
         <v>3.0</v>
       </c>
       <c r="V34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AZ and Lambda for July
</commit_message>
<xml_diff>
--- a/tables/2021-06/sup_table_overview_Jun.xlsx
+++ b/tables/2021-06/sup_table_overview_Jun.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="254">
   <si>
     <t>Population size</t>
   </si>
@@ -176,31 +176,31 @@
     <t>TI</t>
   </si>
   <si>
-    <t>0.70 (0.61-0.80)</t>
-  </si>
-  <si>
-    <t>0.80 (0.52-1.25)</t>
-  </si>
-  <si>
-    <t>0.71 (0.54-0.97)</t>
-  </si>
-  <si>
-    <t>0.80 (0.35-1.59)</t>
-  </si>
-  <si>
-    <t>0.66 (0.50-0.93)</t>
-  </si>
-  <si>
-    <t>0.94 (0.55-1.42)</t>
-  </si>
-  <si>
-    <t>0.70 (0.41-0.98)</t>
+    <t>0.71 (0.62-0.80)</t>
+  </si>
+  <si>
+    <t>0.79 (0.52-1.25)</t>
+  </si>
+  <si>
+    <t>0.71 (0.54-0.98)</t>
+  </si>
+  <si>
+    <t>0.79 (0.36-1.57)</t>
+  </si>
+  <si>
+    <t>0.66 (0.50-0.94)</t>
+  </si>
+  <si>
+    <t>0.94 (0.56-1.42)</t>
+  </si>
+  <si>
+    <t>0.69 (0.42-0.99)</t>
   </si>
   <si>
     <t>0.74 (0.56-1.06)</t>
   </si>
   <si>
-    <t>0.64 (0.37-0.94)</t>
+    <t>0.63 (0.38-0.94)</t>
   </si>
   <si>
     <t>0.62 (0.23-1.20)</t>
@@ -209,58 +209,58 @@
     <t>0.84 (0.45-1.40)</t>
   </si>
   <si>
-    <t>0.76 (0.54-1.08)</t>
-  </si>
-  <si>
-    <t>0.82 (0.40-1.43)</t>
-  </si>
-  <si>
-    <t>0.86 (0.37-1.56)</t>
+    <t>0.77 (0.54-1.08)</t>
+  </si>
+  <si>
+    <t>0.82 (0.39-1.44)</t>
+  </si>
+  <si>
+    <t>0.86 (0.38-1.56)</t>
   </si>
   <si>
     <t>0.88 (0.50-1.38)</t>
   </si>
   <si>
-    <t>0.72 (0.28-1.54)</t>
-  </si>
-  <si>
-    <t>0.71 (0.48-1.14)</t>
+    <t>0.71 (0.28-1.55)</t>
+  </si>
+  <si>
+    <t>0.72 (0.48-1.16)</t>
   </si>
   <si>
     <t>0.60 (0.11-1.56)</t>
   </si>
   <si>
-    <t>0.60 (0.15-1.32)</t>
+    <t>0.60 (0.14-1.34)</t>
   </si>
   <si>
     <t>0.78 (0.52-1.05)</t>
   </si>
   <si>
-    <t>0.58 (0.00-2.09)</t>
-  </si>
-  <si>
-    <t>0.98 (0.53-1.61)</t>
-  </si>
-  <si>
-    <t>0.73 (0.34-1.44)</t>
+    <t>0.56 (0.00-2.13)</t>
+  </si>
+  <si>
+    <t>0.99 (0.53-1.63)</t>
+  </si>
+  <si>
+    <t>0.73 (0.33-1.43)</t>
   </si>
   <si>
     <t>0.42 (0.00-1.17)</t>
   </si>
   <si>
-    <t>0.79 (0.21-1.73)</t>
+    <t>0.80 (0.21-1.75)</t>
   </si>
   <si>
     <t>0.81 (0.22-1.81)</t>
   </si>
   <si>
-    <t>0.61 (0.46-0.83)</t>
-  </si>
-  <si>
-    <t>0.76 (0.33-1.58)</t>
-  </si>
-  <si>
-    <t>0.76 (0.48-1.27)</t>
+    <t>0.61 (0.45-0.83)</t>
+  </si>
+  <si>
+    <t>0.76 (0.32-1.58)</t>
+  </si>
+  <si>
+    <t>0.76 (0.48-1.26)</t>
   </si>
   <si>
     <t>0.78 (0.64-0.92)</t>
@@ -269,7 +269,7 @@
     <t>0.89 (0.51-1.34)</t>
   </si>
   <si>
-    <t>0.90 (0.59-1.29)</t>
+    <t>0.90 (0.59-1.30)</t>
   </si>
   <si>
     <t>1.45</t>
@@ -296,13 +296,13 @@
     <t>1.33</t>
   </si>
   <si>
-    <t>2.10</t>
+    <t>2.11</t>
   </si>
   <si>
     <t>3.88</t>
   </si>
   <si>
-    <t>1.13</t>
+    <t>1.12</t>
   </si>
   <si>
     <t>1.23</t>
@@ -320,7 +320,7 @@
     <t>2.37</t>
   </si>
   <si>
-    <t>1.52</t>
+    <t>1.51</t>
   </si>
   <si>
     <t>4.64</t>
@@ -356,7 +356,7 @@
     <t>2.26</t>
   </si>
   <si>
-    <t>1.21</t>
+    <t>1.22</t>
   </si>
   <si>
     <t>1.10</t>
@@ -368,10 +368,10 @@
     <t>0.74</t>
   </si>
   <si>
-    <t>21.1</t>
-  </si>
-  <si>
-    <t>24.3</t>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>24.4</t>
   </si>
   <si>
     <t>31.7</t>
@@ -380,16 +380,16 @@
     <t>7.7</t>
   </si>
   <si>
-    <t>19.8</t>
+    <t>19.9</t>
   </si>
   <si>
     <t>30.2</t>
   </si>
   <si>
-    <t>17.6</t>
-  </si>
-  <si>
-    <t>30.5</t>
+    <t>17.8</t>
+  </si>
+  <si>
+    <t>30.9</t>
   </si>
   <si>
     <t>0.3</t>
@@ -398,19 +398,19 @@
     <t>3.7</t>
   </si>
   <si>
-    <t>39.5</t>
-  </si>
-  <si>
-    <t>17.2</t>
+    <t>39.8</t>
+  </si>
+  <si>
+    <t>17.5</t>
   </si>
   <si>
     <t>82.9</t>
   </si>
   <si>
-    <t>45.2</t>
-  </si>
-  <si>
-    <t>45.3</t>
+    <t>46.5</t>
+  </si>
+  <si>
+    <t>45.0</t>
   </si>
   <si>
     <t>8.3</t>
@@ -440,7 +440,7 @@
     <t>9.1</t>
   </si>
   <si>
-    <t>23.3</t>
+    <t>23.4</t>
   </si>
   <si>
     <t>17.0</t>
@@ -452,19 +452,19 @@
     <t>19.3</t>
   </si>
   <si>
-    <t>20.5</t>
-  </si>
-  <si>
-    <t>4.8</t>
+    <t>20.7</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
   <si>
     <t>38.5</t>
   </si>
   <si>
-    <t>70.9 (68.6-73.2)</t>
-  </si>
-  <si>
-    <t>60.2 (55.2-65.0)</t>
+    <t>70.5 (68.2-72.7)</t>
+  </si>
+  <si>
+    <t>59.8 (54.8-64.6)</t>
   </si>
   <si>
     <t>52.4 (44.5-60.3)</t>
@@ -473,16 +473,16 @@
     <t>63.6 (30.8-89.1)</t>
   </si>
   <si>
-    <t>61.0 (52.3-69.3)</t>
+    <t>59.9 (51.1-68.1)</t>
   </si>
   <si>
     <t>72.7 (62.2-81.7)</t>
   </si>
   <si>
-    <t>68.9 (61.9-75.4)</t>
-  </si>
-  <si>
-    <t>68.4 (61.3-75.0)</t>
+    <t>67.9 (60.8-74.3)</t>
+  </si>
+  <si>
+    <t>67.4 (60.2-74.0)</t>
   </si>
   <si>
     <t>-</t>
@@ -491,16 +491,16 @@
     <t>100.0 (47.8-100.0)</t>
   </si>
   <si>
-    <t>79.4 (74.9-83.4)</t>
-  </si>
-  <si>
-    <t>88.9 (79.3-95.1)</t>
+    <t>79.0 (74.5-83.1)</t>
+  </si>
+  <si>
+    <t>87.7 (77.9-94.2)</t>
   </si>
   <si>
     <t>85.1 (78.1-90.5)</t>
   </si>
   <si>
-    <t>68.6 (56.4-79.1)</t>
+    <t>68.1 (56.0-78.6)</t>
   </si>
   <si>
     <t>70.4 (59.2-80.0)</t>
@@ -515,13 +515,13 @@
     <t>78.1 (66.0-87.5)</t>
   </si>
   <si>
-    <t>77.5 (73.3-81.4)</t>
+    <t>77.4 (73.1-81.3)</t>
   </si>
   <si>
     <t>75.0 (19.4-99.4)</t>
   </si>
   <si>
-    <t>83.5 (76.8-89.0)</t>
+    <t>83.0 (76.3-88.5)</t>
   </si>
   <si>
     <t>81.2 (54.4-96.0)</t>
@@ -533,10 +533,10 @@
     <t>73.5 (67.1-79.3)</t>
   </si>
   <si>
-    <t>53.8 (42.2-65.0)</t>
-  </si>
-  <si>
-    <t>60.0 (26.2-87.8)</t>
+    <t>53.1 (41.7-64.3)</t>
+  </si>
+  <si>
+    <t>54.5 (23.4-83.3)</t>
   </si>
   <si>
     <t>52.9 (40.6-64.9)</t>
@@ -545,7 +545,7 @@
     <t>0.8 (0.4-1.4)</t>
   </si>
   <si>
-    <t>1.3 (0.4-2.9)</t>
+    <t>1.2 (0.4-2.9)</t>
   </si>
   <si>
     <t>1.8 (0.4-5.3)</t>
@@ -554,16 +554,16 @@
     <t>1.5 (0.2-5.2)</t>
   </si>
   <si>
+    <t>1.5 (0.3-4.4)</t>
+  </si>
+  <si>
     <t>1.6 (0.3-4.5)</t>
   </si>
   <si>
-    <t>1.6 (0.3-4.6)</t>
-  </si>
-  <si>
     <t>0.3 (0.0-1.5)</t>
   </si>
   <si>
-    <t>1.4 (0.0-7.5)</t>
+    <t>1.4 (0.0-7.4)</t>
   </si>
   <si>
     <t>0.9 (0.3-2.4)</t>
@@ -575,7 +575,7 @@
     <t>0.9 (0.1-3.3)</t>
   </si>
   <si>
-    <t>2.1 (1.4-2.9)</t>
+    <t>2.0 (1.4-2.9)</t>
   </si>
   <si>
     <t>1.0 (0.3-2.5)</t>
@@ -584,10 +584,10 @@
     <t>2.3 (0.3-8.0)</t>
   </si>
   <si>
-    <t>2.1 (0.6-5.2)</t>
-  </si>
-  <si>
-    <t>2.1 (0.6-5.4)</t>
+    <t>2.0 (0.6-5.1)</t>
+  </si>
+  <si>
+    <t>2.1 (0.6-5.3)</t>
   </si>
   <si>
     <t>1.1 (0.3-2.8)</t>
@@ -596,7 +596,7 @@
     <t>1.4 (0.2-5.0)</t>
   </si>
   <si>
-    <t>2.9 (0.3-9.9)</t>
+    <t>2.8 (0.3-9.7)</t>
   </si>
   <si>
     <t>3.4 (0.7-9.7)</t>
@@ -617,16 +617,16 @@
     <t>2.3 (0.8-5.3)</t>
   </si>
   <si>
-    <t>5.0 (1.4-12.3)</t>
+    <t>4.9 (1.4-12.2)</t>
   </si>
   <si>
     <t>5.7 (1.6-14.0)</t>
   </si>
   <si>
-    <t>20.6 (18.6-22.7)</t>
-  </si>
-  <si>
-    <t>30.1 (25.6-34.8)</t>
+    <t>20.9 (19.0-23.0)</t>
+  </si>
+  <si>
+    <t>30.2 (25.8-35.0)</t>
   </si>
   <si>
     <t>36.0 (28.6-43.8)</t>
@@ -635,34 +635,34 @@
     <t>36.4 (10.9-69.2)</t>
   </si>
   <si>
-    <t>26.5 (19.3-34.7)</t>
+    <t>27.0 (19.8-35.3)</t>
   </si>
   <si>
     <t>23.9 (15.4-34.1)</t>
   </si>
   <si>
-    <t>20.7 (15.2-27.1)</t>
-  </si>
-  <si>
-    <t>20.9 (15.3-27.4)</t>
+    <t>21.9 (16.4-28.4)</t>
+  </si>
+  <si>
+    <t>22.1 (16.4-28.7)</t>
   </si>
   <si>
     <t>100.0 (2.5-100.0)</t>
   </si>
   <si>
-    <t>17.0 (13.3-21.3)</t>
-  </si>
-  <si>
-    <t>6.9 (2.3-15.5)</t>
+    <t>17.2 (13.5-21.4)</t>
+  </si>
+  <si>
+    <t>8.2 (3.1-17.0)</t>
   </si>
   <si>
     <t>10.6 (6.1-16.9)</t>
   </si>
   <si>
-    <t>25.7 (16.0-37.6)</t>
-  </si>
-  <si>
-    <t>29.6 (20.0-40.8)</t>
+    <t>26.4 (16.7-38.1)</t>
+  </si>
+  <si>
+    <t>28.4 (18.9-39.5)</t>
   </si>
   <si>
     <t>21.8 (13.7-32.0)</t>
@@ -677,13 +677,13 @@
     <t>15.6 (7.8-26.9)</t>
   </si>
   <si>
-    <t>14.7 (11.4-18.4)</t>
+    <t>14.9 (11.6-18.6)</t>
   </si>
   <si>
     <t>25.0 (0.6-80.6)</t>
   </si>
   <si>
-    <t>9.5 (5.4-15.2)</t>
+    <t>10.1 (5.9-15.8)</t>
   </si>
   <si>
     <t>18.8 (4.0-45.6)</t>
@@ -695,22 +695,25 @@
     <t>17.7 (12.8-23.4)</t>
   </si>
   <si>
-    <t>20.0 (11.9-30.4)</t>
-  </si>
-  <si>
-    <t>40.0 (12.2-73.8)</t>
+    <t>21.0 (12.7-31.5)</t>
+  </si>
+  <si>
+    <t>45.5 (16.7-76.6)</t>
   </si>
   <si>
     <t>17.1 (9.2-28.0)</t>
   </si>
   <si>
-    <t>1.7 (1.1-2.4)</t>
+    <t>1.7 (1.1-2.5)</t>
+  </si>
+  <si>
+    <t>2.4 (0.7-6.1)</t>
   </si>
   <si>
     <t>0.7 (0.0-4.0)</t>
   </si>
   <si>
-    <t>1.0 (0.1-3.7)</t>
+    <t>1.0 (0.1-3.6)</t>
   </si>
   <si>
     <t>1.1 (0.1-3.8)</t>
@@ -725,34 +728,37 @@
     <t>1.4 (0.3-4.0)</t>
   </si>
   <si>
-    <t>17.5 (9.9-27.6)</t>
+    <t>17.3 (9.8-27.3)</t>
   </si>
   <si>
     <t>20.0 (11.4-31.3)</t>
   </si>
   <si>
-    <t>3.9 (3.0-5.0)</t>
+    <t>4.0 (3.0-5.0)</t>
   </si>
   <si>
     <t>6.5 (4.3-9.4)</t>
   </si>
   <si>
-    <t>7.9 (4.3-13.2)</t>
-  </si>
-  <si>
-    <t>8.8 (4.6-14.9)</t>
+    <t>7.3 (3.8-12.4)</t>
+  </si>
+  <si>
+    <t>9.5 (5.1-15.7)</t>
   </si>
   <si>
     <t>1.1 (0.0-6.2)</t>
   </si>
   <si>
-    <t>5.7 (2.9-10.0)</t>
-  </si>
-  <si>
-    <t>5.9 (3.0-10.3)</t>
-  </si>
-  <si>
-    <t>1.4 (0.4-3.2)</t>
+    <t>5.6 (2.8-9.8)</t>
+  </si>
+  <si>
+    <t>5.8 (2.9-10.1)</t>
+  </si>
+  <si>
+    <t>1.6 (0.6-3.5)</t>
+  </si>
+  <si>
+    <t>1.2 (0.0-6.7)</t>
   </si>
   <si>
     <t>1.6 (0.0-8.4)</t>
@@ -764,7 +770,7 @@
     <t>4.2 (1.9-7.8)</t>
   </si>
   <si>
-    <t>3.8 (0.8-10.6)</t>
+    <t>3.7 (0.8-10.4)</t>
   </si>
   <si>
     <t>4.3 (0.9-12.0)</t>
@@ -892,25 +898,25 @@
         <v>8606033.0</v>
       </c>
       <c r="C2" t="n">
-        <v>7367.0</v>
+        <v>7370.0</v>
       </c>
       <c r="D2" t="n">
-        <v>183.0</v>
+        <v>184.0</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
       </c>
       <c r="F2" t="n">
-        <v>608296.0</v>
+        <v>608851.0</v>
       </c>
       <c r="G2" t="n">
-        <v>7068.0</v>
+        <v>7075.0</v>
       </c>
       <c r="H2" t="s">
         <v>86</v>
       </c>
       <c r="I2" t="n">
-        <v>1557.0</v>
+        <v>1566.0</v>
       </c>
       <c r="J2" t="s">
         <v>118</v>
@@ -934,22 +940,22 @@
         <v>187</v>
       </c>
       <c r="Q2" t="n">
-        <v>321.0</v>
+        <v>328.0</v>
       </c>
       <c r="R2" t="s">
         <v>203</v>
       </c>
       <c r="S2" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="T2" t="s">
         <v>230</v>
       </c>
       <c r="U2" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="V2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
@@ -960,31 +966,31 @@
         <v>1831247.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1639.0</v>
+        <v>1640.0</v>
       </c>
       <c r="D3" t="n">
-        <v>42.0</v>
+        <v>192.0</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
       </c>
       <c r="F3" t="n">
-        <v>169414.0</v>
+        <v>169424.0</v>
       </c>
       <c r="G3" t="n">
-        <v>9251.0</v>
+        <v>9252.0</v>
       </c>
       <c r="H3" t="s">
         <v>87</v>
       </c>
       <c r="I3" t="n">
-        <v>399.0</v>
+        <v>400.0</v>
       </c>
       <c r="J3" t="s">
         <v>119</v>
       </c>
       <c r="K3" t="n">
-        <v>240.0</v>
+        <v>239.0</v>
       </c>
       <c r="L3" t="s">
         <v>150</v>
@@ -1002,22 +1008,22 @@
         <v>188</v>
       </c>
       <c r="Q3" t="n">
-        <v>120.0</v>
+        <v>121.0</v>
       </c>
       <c r="R3" t="s">
         <v>204</v>
       </c>
       <c r="S3" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="T3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="U3" t="n">
         <v>26.0</v>
       </c>
       <c r="V3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4">
@@ -1076,16 +1082,16 @@
         <v>205</v>
       </c>
       <c r="S4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="T4" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="U4" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="V4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
@@ -1105,7 +1111,7 @@
         <v>57</v>
       </c>
       <c r="F5" t="n">
-        <v>13098.0</v>
+        <v>13097.0</v>
       </c>
       <c r="G5" t="n">
         <v>7421.0</v>
@@ -1164,7 +1170,7 @@
         <v>805098.0</v>
       </c>
       <c r="C6" t="n">
-        <v>687.0</v>
+        <v>688.0</v>
       </c>
       <c r="D6" t="n">
         <v>183.0</v>
@@ -1173,7 +1179,7 @@
         <v>58</v>
       </c>
       <c r="F6" t="n">
-        <v>79117.0</v>
+        <v>79119.0</v>
       </c>
       <c r="G6" t="n">
         <v>9827.0</v>
@@ -1182,13 +1188,13 @@
         <v>90</v>
       </c>
       <c r="I6" t="n">
-        <v>136.0</v>
+        <v>137.0</v>
       </c>
       <c r="J6" t="s">
         <v>122</v>
       </c>
       <c r="K6" t="n">
-        <v>83.0</v>
+        <v>82.0</v>
       </c>
       <c r="L6" t="s">
         <v>153</v>
@@ -1206,7 +1212,7 @@
         <v>179</v>
       </c>
       <c r="Q6" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="R6" t="s">
         <v>207</v>
@@ -1215,13 +1221,13 @@
         <v>1.0</v>
       </c>
       <c r="T6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="U6" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="V6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7">
@@ -1241,10 +1247,10 @@
         <v>59</v>
       </c>
       <c r="F7" t="n">
-        <v>27330.0</v>
+        <v>27339.0</v>
       </c>
       <c r="G7" t="n">
-        <v>7910.0</v>
+        <v>7912.0</v>
       </c>
       <c r="H7" t="s">
         <v>91</v>
@@ -1289,7 +1295,7 @@
         <v>1.0</v>
       </c>
       <c r="V7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8">
@@ -1300,25 +1306,25 @@
         <v>1434841.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1098.0</v>
+        <v>1099.0</v>
       </c>
       <c r="D8" t="n">
-        <v>36.0</v>
+        <v>164.0</v>
       </c>
       <c r="E8" t="s">
         <v>60</v>
       </c>
       <c r="F8" t="n">
-        <v>76427.0</v>
+        <v>76485.0</v>
       </c>
       <c r="G8" t="n">
-        <v>5327.0</v>
+        <v>5331.0</v>
       </c>
       <c r="H8" t="s">
         <v>92</v>
       </c>
       <c r="I8" t="n">
-        <v>193.0</v>
+        <v>196.0</v>
       </c>
       <c r="J8" t="s">
         <v>124</v>
@@ -1342,7 +1348,7 @@
         <v>190</v>
       </c>
       <c r="Q8" t="n">
-        <v>40.0</v>
+        <v>43.0</v>
       </c>
       <c r="R8" t="s">
         <v>209</v>
@@ -1351,13 +1357,13 @@
         <v>2.0</v>
       </c>
       <c r="T8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="U8" t="n">
         <v>11.0</v>
       </c>
       <c r="V8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
@@ -1377,16 +1383,16 @@
         <v>61</v>
       </c>
       <c r="F9" t="n">
-        <v>52675.0</v>
+        <v>52731.0</v>
       </c>
       <c r="G9" t="n">
-        <v>5067.0</v>
+        <v>5073.0</v>
       </c>
       <c r="H9" t="s">
         <v>93</v>
       </c>
       <c r="I9" t="n">
-        <v>187.0</v>
+        <v>190.0</v>
       </c>
       <c r="J9" t="s">
         <v>125</v>
@@ -1410,7 +1416,7 @@
         <v>191</v>
       </c>
       <c r="Q9" t="n">
-        <v>39.0</v>
+        <v>42.0</v>
       </c>
       <c r="R9" t="s">
         <v>210</v>
@@ -1419,13 +1425,13 @@
         <v>2.0</v>
       </c>
       <c r="T9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="U9" t="n">
         <v>11.0</v>
       </c>
       <c r="V9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10">
@@ -1436,19 +1442,19 @@
         <v>321783.0</v>
       </c>
       <c r="C10" t="n">
-        <v>350.0</v>
+        <v>351.0</v>
       </c>
       <c r="D10" t="n">
-        <v>233.0</v>
+        <v>234.0</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
       </c>
       <c r="F10" t="n">
-        <v>19651.0</v>
+        <v>19653.0</v>
       </c>
       <c r="G10" t="n">
-        <v>6107.0</v>
+        <v>6108.0</v>
       </c>
       <c r="H10" t="s">
         <v>94</v>
@@ -1572,31 +1578,31 @@
         <v>1446404.0</v>
       </c>
       <c r="C12" t="n">
-        <v>922.0</v>
+        <v>923.0</v>
       </c>
       <c r="D12" t="n">
-        <v>30.0</v>
+        <v>137.0</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
       </c>
       <c r="F12" t="n">
-        <v>95122.0</v>
+        <v>95776.0</v>
       </c>
       <c r="G12" t="n">
-        <v>6576.0</v>
+        <v>6622.0</v>
       </c>
       <c r="H12" t="s">
         <v>96</v>
       </c>
       <c r="I12" t="n">
-        <v>364.0</v>
+        <v>367.0</v>
       </c>
       <c r="J12" t="s">
         <v>128</v>
       </c>
       <c r="K12" t="n">
-        <v>289.0</v>
+        <v>290.0</v>
       </c>
       <c r="L12" t="s">
         <v>159</v>
@@ -1614,7 +1620,7 @@
         <v>192</v>
       </c>
       <c r="Q12" t="n">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="R12" t="s">
         <v>212</v>
@@ -1623,13 +1629,13 @@
         <v>3.0</v>
       </c>
       <c r="T12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="U12" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="V12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13">
@@ -1649,16 +1655,16 @@
         <v>65</v>
       </c>
       <c r="F13" t="n">
-        <v>39600.0</v>
+        <v>39655.0</v>
       </c>
       <c r="G13" t="n">
-        <v>5774.0</v>
+        <v>5782.0</v>
       </c>
       <c r="H13" t="s">
         <v>97</v>
       </c>
       <c r="I13" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
       <c r="J13" t="s">
         <v>129</v>
@@ -1682,7 +1688,7 @@
         <v>157</v>
       </c>
       <c r="Q13" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="R13" t="s">
         <v>213</v>
@@ -1717,10 +1723,10 @@
         <v>66</v>
       </c>
       <c r="F14" t="n">
-        <v>19590.0</v>
+        <v>19594.0</v>
       </c>
       <c r="G14" t="n">
-        <v>6768.0</v>
+        <v>6769.0</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -1794,13 +1800,13 @@
         <v>99</v>
       </c>
       <c r="I15" t="n">
-        <v>70.0</v>
+        <v>72.0</v>
       </c>
       <c r="J15" t="s">
         <v>131</v>
       </c>
       <c r="K15" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
       <c r="L15" t="s">
         <v>162</v>
@@ -1818,7 +1824,7 @@
         <v>194</v>
       </c>
       <c r="Q15" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="R15" t="s">
         <v>215</v>
@@ -1844,22 +1850,22 @@
         <v>275247.0</v>
       </c>
       <c r="C16" t="n">
-        <v>179.0</v>
+        <v>180.0</v>
       </c>
       <c r="D16" t="n">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
       <c r="E16" t="s">
         <v>68</v>
       </c>
       <c r="F16" t="n">
-        <v>15603.0</v>
+        <v>16198.0</v>
       </c>
       <c r="G16" t="n">
-        <v>5669.0</v>
+        <v>5885.0</v>
       </c>
       <c r="H16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I16" t="n">
         <v>81.0</v>
@@ -1886,7 +1892,7 @@
         <v>157</v>
       </c>
       <c r="Q16" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="R16" t="s">
         <v>216</v>
@@ -1898,10 +1904,10 @@
         <v>157</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V16" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17">
@@ -1915,16 +1921,16 @@
         <v>1054.0</v>
       </c>
       <c r="D17" t="n">
-        <v>60.0</v>
+        <v>276.0</v>
       </c>
       <c r="E17" t="s">
         <v>69</v>
       </c>
       <c r="F17" t="n">
-        <v>60402.0</v>
+        <v>60417.0</v>
       </c>
       <c r="G17" t="n">
-        <v>7375.0</v>
+        <v>7377.0</v>
       </c>
       <c r="H17" t="s">
         <v>100</v>
@@ -1969,7 +1975,7 @@
         <v>1.0</v>
       </c>
       <c r="V17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18">
@@ -1989,7 +1995,7 @@
         <v>70</v>
       </c>
       <c r="F18" t="n">
-        <v>19316.0</v>
+        <v>19319.0</v>
       </c>
       <c r="G18" t="n">
         <v>4676.0</v>
@@ -2057,10 +2063,10 @@
         <v>71</v>
       </c>
       <c r="F19" t="n">
-        <v>3490.0</v>
+        <v>3502.0</v>
       </c>
       <c r="G19" t="n">
-        <v>8100.0</v>
+        <v>8128.0</v>
       </c>
       <c r="H19" t="s">
         <v>102</v>
@@ -2241,7 +2247,7 @@
         <v>1.0</v>
       </c>
       <c r="V21" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22">
@@ -2391,22 +2397,22 @@
         <v>2263.0</v>
       </c>
       <c r="D24" t="n">
-        <v>42.0</v>
+        <v>192.0</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
       <c r="F24" t="n">
-        <v>160798.0</v>
+        <v>160589.0</v>
       </c>
       <c r="G24" t="n">
-        <v>6371.0</v>
+        <v>6362.0</v>
       </c>
       <c r="H24" t="s">
         <v>107</v>
       </c>
       <c r="I24" t="n">
-        <v>423.0</v>
+        <v>424.0</v>
       </c>
       <c r="J24" t="s">
         <v>140</v>
@@ -2430,7 +2436,7 @@
         <v>197</v>
       </c>
       <c r="Q24" t="n">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="R24" t="s">
         <v>221</v>
@@ -2439,7 +2445,7 @@
         <v>3.0</v>
       </c>
       <c r="T24" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="U24" t="n">
         <v>13.0</v>
@@ -2678,7 +2684,7 @@
         <v>111</v>
       </c>
       <c r="I28" t="n">
-        <v>158.0</v>
+        <v>159.0</v>
       </c>
       <c r="J28" t="s">
         <v>142</v>
@@ -2702,7 +2708,7 @@
         <v>198</v>
       </c>
       <c r="Q28" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="R28" t="s">
         <v>223</v>
@@ -2737,10 +2743,10 @@
         <v>81</v>
       </c>
       <c r="F29" t="n">
-        <v>4583.0</v>
+        <v>4584.0</v>
       </c>
       <c r="G29" t="n">
-        <v>5565.0</v>
+        <v>5567.0</v>
       </c>
       <c r="H29" t="s">
         <v>112</v>
@@ -2805,7 +2811,7 @@
         <v>82</v>
       </c>
       <c r="F30" t="n">
-        <v>11948.0</v>
+        <v>11947.0</v>
       </c>
       <c r="G30" t="n">
         <v>4274.0</v>
@@ -2853,7 +2859,7 @@
         <v>2.0</v>
       </c>
       <c r="V30" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31">
@@ -2873,10 +2879,10 @@
         <v>83</v>
       </c>
       <c r="F31" t="n">
-        <v>111619.0</v>
+        <v>111410.0</v>
       </c>
       <c r="G31" t="n">
-        <v>7251.0</v>
+        <v>7238.0</v>
       </c>
       <c r="H31" t="s">
         <v>114</v>
@@ -2915,13 +2921,13 @@
         <v>3.0</v>
       </c>
       <c r="T31" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="U31" t="n">
         <v>9.0</v>
       </c>
       <c r="V31" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32">
@@ -2935,22 +2941,22 @@
         <v>391.0</v>
       </c>
       <c r="D32" t="n">
-        <v>33.0</v>
+        <v>152.0</v>
       </c>
       <c r="E32" t="s">
         <v>84</v>
       </c>
       <c r="F32" t="n">
-        <v>46133.0</v>
+        <v>46160.0</v>
       </c>
       <c r="G32" t="n">
-        <v>8380.0</v>
+        <v>8385.0</v>
       </c>
       <c r="H32" t="s">
         <v>115</v>
       </c>
       <c r="I32" t="n">
-        <v>80.0</v>
+        <v>81.0</v>
       </c>
       <c r="J32" t="s">
         <v>146</v>
@@ -2974,7 +2980,7 @@
         <v>201</v>
       </c>
       <c r="Q32" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="R32" t="s">
         <v>227</v>
@@ -2983,13 +2989,13 @@
         <v>14.0</v>
       </c>
       <c r="T32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="U32" t="n">
         <v>3.0</v>
       </c>
       <c r="V32" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33">
@@ -3009,7 +3015,7 @@
         <v>85</v>
       </c>
       <c r="F33" t="n">
-        <v>13529.0</v>
+        <v>13530.0</v>
       </c>
       <c r="G33" t="n">
         <v>6798.0</v>
@@ -3018,7 +3024,7 @@
         <v>116</v>
       </c>
       <c r="I33" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J33" t="s">
         <v>147</v>
@@ -3042,7 +3048,7 @@
         <v>157</v>
       </c>
       <c r="Q33" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="R33" t="s">
         <v>228</v>
@@ -3077,10 +3083,10 @@
         <v>68</v>
       </c>
       <c r="F34" t="n">
-        <v>32604.0</v>
+        <v>32630.0</v>
       </c>
       <c r="G34" t="n">
-        <v>9276.0</v>
+        <v>9283.0</v>
       </c>
       <c r="H34" t="s">
         <v>117</v>
@@ -3119,13 +3125,13 @@
         <v>14.0</v>
       </c>
       <c r="T34" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="U34" t="n">
         <v>3.0</v>
       </c>
       <c r="V34" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>